<commit_message>
Added cell in spreadsheet for failure test on start time column
</commit_message>
<xml_diff>
--- a/spec/support/roInvalidTimeSlotStartTime.xlsx
+++ b/spec/support/roInvalidTimeSlotStartTime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566A5754-79F8-E840-8EDC-36FB4D3461EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12118D9A-AAC3-1849-9374-85DF706A88CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13040" yWindow="460" windowWidth="25360" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="130">
   <si>
     <t>Example</t>
   </si>
@@ -1279,6 +1279,7 @@
     <xf numFmtId="49" fontId="16" fillId="13" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1309,7 +1310,6 @@
     <xf numFmtId="49" fontId="15" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2524,19 +2524,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -6238,10 +6238,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="81"/>
       <c r="C1" s="40"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
@@ -6342,7 +6342,7 @@
   <dimension ref="A1:IV98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6358,16 +6358,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="83"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="47"/>
       <c r="J1" s="47"/>
       <c r="K1" s="47"/>
@@ -6380,12 +6380,12 @@
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
       <c r="D2" s="63"/>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
       <c r="K2" s="29"/>
@@ -6475,7 +6475,7 @@
       <c r="G5" s="29">
         <v>30</v>
       </c>
-      <c r="H5" s="87">
+      <c r="H5" s="77">
         <v>-1</v>
       </c>
       <c r="I5" s="29"/>
@@ -6535,8 +6535,8 @@
       <c r="G7" s="29">
         <v>30</v>
       </c>
-      <c r="H7" s="76" t="s">
-        <v>128</v>
+      <c r="H7" s="77">
+        <v>15</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>

</xml_diff>